<commit_message>
login icin Cookies sirasi degistirildi.
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resources/senarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resources/senarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
   <si>
     <t>apachipoı-citizen-functionality;create-an-delete-citizenship-from-excel</t>
   </si>
@@ -39,6 +39,12 @@
   </si>
   <si>
     <t>passed</t>
+  </si>
+  <si>
+    <t>login--functionality;login-with-valid-username-and-password</t>
+  </si>
+  <si>
+    <t>16.09.21</t>
   </si>
 </sst>
 </file>
@@ -83,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -243,6 +249,20 @@
         <v>5</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Jenkis icin  ChromeOptions options = new ChromeOptions();eklendi
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resources/senarioStatus.xlsx
+++ b/src/test/java/ApachePOI/resources/senarioStatus.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="11">
   <si>
     <t>apachipoı-citizen-functionality;create-an-delete-citizenship-from-excel</t>
   </si>
@@ -89,7 +89,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -263,6 +263,48 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>